<commit_message>
Typo fix (classic Shettalian move...)
git-svn-id: svn+ssh://svn.code.sf.net/p/open-fvs/code/rFVS@2800 90b89b48-9230-0de4-5065-812dd12741b8
</commit_message>
<xml_diff>
--- a/shinyFVSOnlineDev/databaseDescription.xlsx
+++ b/shinyFVSOnlineDev/databaseDescription.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FVSOnlocal\Stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Open-FVS\rFVS\shinyFVSOnlineDev\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="36" activeTab="37"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTableDescriptions" sheetId="1" r:id="rId1"/>
@@ -4888,9 +4888,6 @@
     <t>contains a summary of the trees per acre , by species, of ingrowth predicted by the full establishment model for a given cycle.</t>
   </si>
   <si>
-    <t>contains a summry by species of the trees per acre, percentage of total, and average height for all trees, best trees, and trees less than 3 inched in diameter that regenerated during a given tally.</t>
-  </si>
-  <si>
     <t>contains a summary of the percentage of the plots that received mechanical, burning, or no site preparation, and in which year.</t>
   </si>
   <si>
@@ -5241,6 +5238,9 @@
   </si>
   <si>
     <t>Trees per acre of the best trees regenerating during a given tally, minus any sprouts, for a given species. Best trees are the "desirable" trees most likely to survive and contribute to yield &amp; future stand development.</t>
+  </si>
+  <si>
+    <t>contains a summary by species of the trees per acre, percentage of total, and average height for all trees, best trees, and trees less than 3 inched in diameter that regenerated during a given tally.</t>
   </si>
 </sst>
 </file>
@@ -5639,8 +5639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK45"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5903,7 +5903,7 @@
         <v>1567</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -5911,7 +5911,7 @@
         <v>1568</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -5919,7 +5919,7 @@
         <v>1569</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -5927,7 +5927,7 @@
         <v>1570</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -5935,7 +5935,7 @@
         <v>1571</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1577</v>
+        <v>1694</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -14161,63 +14161,63 @@
         <v>81</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>100</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
     </row>
   </sheetData>
@@ -14298,142 +14298,142 @@
     </row>
     <row r="5" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>81</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="C6" t="s">
         <v>100</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>1602</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>1603</v>
-      </c>
       <c r="C7" t="s">
         <v>100</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="C8" t="s">
         <v>100</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="C9" t="s">
         <v>115</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="C10" t="s">
         <v>115</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="C11" t="s">
         <v>100</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="C12" t="s">
         <v>100</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="C13" t="s">
         <v>100</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C14" t="s">
         <v>100</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
     </row>
   </sheetData>
@@ -14510,7 +14510,7 @@
         <v>115</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -14524,35 +14524,35 @@
         <v>81</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>1620</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>1621</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>115</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>1622</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="13" t="s">
         <v>1623</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>1624</v>
-      </c>
       <c r="D7" s="7" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
     </row>
   </sheetData>
@@ -14619,86 +14619,86 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="B4" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>115</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="B6" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B7" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="B8" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D8" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="B9" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
     </row>
   </sheetData>
@@ -14765,58 +14765,58 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B4" t="s">
         <v>1645</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1646</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="B5" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="C5" t="s">
         <v>115</v>
       </c>
       <c r="D5" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B6" t="s">
         <v>1651</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1652</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B7" t="s">
         <v>1653</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1654</v>
       </c>
       <c r="C7" t="s">
         <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
     </row>
   </sheetData>
@@ -14828,7 +14828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -14892,35 +14892,35 @@
         <v>115</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>1657</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>1658</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>1659</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>1659</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>1660</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>1661</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>115</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -14934,105 +14934,105 @@
         <v>81</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>115</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>115</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>115</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>1672</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>1673</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>1674</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>115</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>115</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
     </row>
   </sheetData>
@@ -15108,21 +15108,21 @@
         <v>115</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
+        <v>1683</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>1684</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="C5" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>1685</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>1686</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -15136,21 +15136,21 @@
         <v>81</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>1688</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>1689</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>115</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated the SnagSum table's default diameter range values in the description.
git-svn-id: svn+ssh://svn.code.sf.net/p/open-fvs/code/rFVS@2981 90b89b48-9230-0de4-5065-812dd12741b8
</commit_message>
<xml_diff>
--- a/shinyFVSOnlineDev/databaseDescription.xlsx
+++ b/shinyFVSOnlineDev/databaseDescription.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FVS\Project_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michaelashettles\Documents\Program of Work\POW 17\Online FVS\fvssetup\Fvsbin\FVSProjects\Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55A794D-396F-4682-A019-D71BA02C5866}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D473678-B052-4EC8-A86E-B6056907ECAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" firstSheet="25" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" firstSheet="21" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTableDescriptions" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4448" uniqueCount="1848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4448" uniqueCount="1851">
   <si>
     <t>Table</t>
   </si>
@@ -5577,42 +5577,6 @@
     <t>Average large-tree diameter growth, or small-tree height growth, scale factors for a species within a given stand. Applied before calibration, these multipliers are used to permanently change the model to a different mean response level.</t>
   </si>
   <si>
-    <t>Hard snags in size class 1 (default=0.0-12.0")</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 1 (default=0.0-12.0")</t>
-  </si>
-  <si>
-    <t>Hard snags in size class 2 (default=12.0-18.0")</t>
-  </si>
-  <si>
-    <t>Hard snags in size class 3 (default=18.0-24.0")</t>
-  </si>
-  <si>
-    <t>Hard snags in size class 4 (default=24.0-30.0")</t>
-  </si>
-  <si>
-    <t>Hard snags in size class 5 (default=30.0-36.0")</t>
-  </si>
-  <si>
-    <t>Hard snags in size class 6 (default=36.0"+)</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 2 (default=12.0-18.0")</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 3 (default=18.0-24.0")</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 4 (default=24.0-30.0")</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 5 (default=30.0-36.0")</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 6 (default=36.0"+)</t>
-  </si>
-  <si>
     <t>FVS_Potfire_East</t>
   </si>
   <si>
@@ -5707,6 +5671,51 @@
   </si>
   <si>
     <t>Basal area per acre (sq ft/acre)</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 1 (default &gt;=0.0")</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 2 (default &gt;=12.0")</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 3 (default &gt;=18.0")</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 4 (default &gt;=24.0")</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 5 (default &gt;=30.0")</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 6 (default &gt;=36.0")</t>
+  </si>
+  <si>
+    <t>Hard snags total (all &gt;=0”)</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 1 (default &gt;=0.0")</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 2 (default &gt;=12.0")</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 3 (default &gt;=18.0")</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 4 (default &gt;=24.0")</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 5 (default &gt;=30.0")</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 6 (default &gt;=36.0")</t>
+  </si>
+  <si>
+    <t>Soft snags total (all &gt;=0”)</t>
+  </si>
+  <si>
+    <t>Hard and soft snags total (all &gt;=0”)</t>
   </si>
 </sst>
 </file>
@@ -6273,7 +6282,7 @@
     </row>
     <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>1816</v>
+        <v>1804</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>1667</v>
@@ -8993,7 +9002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>78</v>
       </c>
@@ -9046,7 +9055,7 @@
         <v>99</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1817</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9060,7 +9069,7 @@
         <v>99</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>1818</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9074,7 +9083,7 @@
         <v>99</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>1819</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9088,7 +9097,7 @@
         <v>99</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>1820</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -9102,7 +9111,7 @@
         <v>99</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>1821</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -9116,7 +9125,7 @@
         <v>99</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>1822</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -9130,7 +9139,7 @@
         <v>99</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>1823</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9144,7 +9153,7 @@
         <v>99</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>1824</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9158,7 +9167,7 @@
         <v>99</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>1825</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -9172,7 +9181,7 @@
         <v>99</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>1826</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -9186,7 +9195,7 @@
         <v>99</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>1827</v>
+        <v>1815</v>
       </c>
     </row>
   </sheetData>
@@ -9581,7 +9590,7 @@
         <v>99</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1828</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -9595,7 +9604,7 @@
         <v>99</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>1829</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -9609,7 +9618,7 @@
         <v>99</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>1830</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -9623,7 +9632,7 @@
         <v>99</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>1831</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9637,7 +9646,7 @@
         <v>99</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>1832</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9651,7 +9660,7 @@
         <v>99</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>1833</v>
+        <v>1821</v>
       </c>
     </row>
   </sheetData>
@@ -12376,8 +12385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:AMK19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12456,7 +12465,7 @@
         <v>99</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1804</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -12470,7 +12479,7 @@
         <v>99</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>1806</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -12484,7 +12493,7 @@
         <v>99</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>1807</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -12498,7 +12507,7 @@
         <v>99</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>1808</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -12512,7 +12521,7 @@
         <v>99</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>1809</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -12526,7 +12535,7 @@
         <v>99</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>1810</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -12540,7 +12549,7 @@
         <v>99</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>764</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -12554,7 +12563,7 @@
         <v>99</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>1805</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -12568,7 +12577,7 @@
         <v>99</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>1811</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -12582,7 +12591,7 @@
         <v>99</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>1812</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -12596,7 +12605,7 @@
         <v>99</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>1813</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -12610,7 +12619,7 @@
         <v>99</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>1814</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -12624,7 +12633,7 @@
         <v>99</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>1815</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -12638,7 +12647,7 @@
         <v>99</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>778</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -12652,12 +12661,12 @@
         <v>99</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>780</v>
+        <v>1850</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13533,7 +13542,7 @@
         <v>99</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>1847</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -13575,7 +13584,7 @@
         <v>99</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>1846</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -13589,7 +13598,7 @@
         <v>99</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>1845</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -13603,7 +13612,7 @@
         <v>99</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>1844</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13617,7 +13626,7 @@
         <v>99</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>1843</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13631,7 +13640,7 @@
         <v>99</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>1842</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13645,7 +13654,7 @@
         <v>99</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>1841</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13659,7 +13668,7 @@
         <v>99</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>1840</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -13673,7 +13682,7 @@
         <v>99</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>1839</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -13687,7 +13696,7 @@
         <v>99</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>1838</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -13701,7 +13710,7 @@
         <v>99</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>1837</v>
+        <v>1825</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>1538</v>
@@ -13746,7 +13755,7 @@
         <v>99</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>1834</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -13760,7 +13769,7 @@
         <v>99</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>1835</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -13774,7 +13783,7 @@
         <v>114</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>1836</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -14252,7 +14261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:AMK20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -16537,7 +16546,7 @@
         <v>99</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>1846</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -16705,7 +16714,7 @@
         <v>114</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>1836</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
FVSOnlineDev: Slight edit to databaseDescription, edited help to correspond to recent changes, help is now in a scrollable window so that the FVSOnline heading is always shown, added "return to top" after every table description is shown.
git-svn-id: svn+ssh://svn.code.sf.net/p/open-fvs/code/rFVS@3033 90b89b48-9230-0de4-5065-812dd12741b8
</commit_message>
<xml_diff>
--- a/shinyFVSOnlineDev/databaseDescription.xlsx
+++ b/shinyFVSOnlineDev/databaseDescription.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="48"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTableDescriptions" sheetId="1" state="visible" r:id="rId2"/>
@@ -948,7 +948,7 @@
     <t xml:space="preserve">Variable n</t>
   </si>
   <si>
-    <t xml:space="preserve">The n compute variable</t>
+    <t xml:space="preserve">The nth compute variable</t>
   </si>
   <si>
     <t xml:space="preserve">Stand identification</t>
@@ -6376,7 +6376,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="49.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="49.87"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
   <sheetData>
@@ -6615,7 +6615,7 @@
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="27.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="27.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="80.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
@@ -7095,7 +7095,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="26.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="80.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
@@ -7573,7 +7573,7 @@
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="80.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
@@ -9104,8 +9104,8 @@
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="32.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="32.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="61.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
@@ -9418,7 +9418,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="55.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9.13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="2" width="8.57"/>
   </cols>
   <sheetData>
@@ -9940,9 +9940,9 @@
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="26.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="41.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="41.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
   <sheetData>
@@ -10153,7 +10153,7 @@
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="70.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
@@ -10604,7 +10604,7 @@
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="41.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="70.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
@@ -11310,8 +11310,8 @@
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="27.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="71.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
@@ -11637,7 +11637,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="34.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="45.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="45.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
   <sheetData>
@@ -11917,9 +11917,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="7" width="28.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="7" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="9.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="67.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="67.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
   <sheetData>
@@ -12228,8 +12228,8 @@
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="61.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
@@ -13443,7 +13443,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="31.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="34"/>
@@ -13899,7 +13899,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="40.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="80.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
@@ -14069,7 +14069,7 @@
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="7" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="67.29"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
@@ -14294,7 +14294,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="26.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="29.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="81.57"/>
@@ -14605,7 +14605,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="7" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="7" width="23.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="49.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
@@ -14860,7 +14860,7 @@
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="52.85"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
@@ -15117,7 +15117,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="37.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="60.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="60.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
   <sheetData>
@@ -15469,8 +15469,8 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="53.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="67.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="67.41"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
   <sheetData>
@@ -15958,7 +15958,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.29"/>
@@ -16113,9 +16113,9 @@
       <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="77.29"/>
   </cols>
@@ -16338,7 +16338,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.7"/>
@@ -16467,10 +16467,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="31.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="44.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="44.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
   <sheetData>
@@ -16916,7 +16916,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.29"/>
@@ -17071,7 +17071,7 @@
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.29"/>
@@ -17198,11 +17198,11 @@
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="72.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="72.02"/>
   </cols>
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17423,11 +17423,11 @@
       <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="72.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="72.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17755,7 +17755,7 @@
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="17.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="60.29"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
@@ -20233,11 +20233,11 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.82"/>
@@ -20402,7 +20402,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="30.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="37.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="37.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
   <sheetData>
@@ -20848,9 +20848,9 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.71"/>
@@ -21200,9 +21200,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.71"/>
@@ -22265,7 +22265,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="31.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="44.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="44.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>
   <sheetData>
@@ -22707,8 +22707,8 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22804,7 +22804,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>262</v>
       </c>
@@ -22842,9 +22842,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="30.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="64.7"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="2" width="8.57"/>
   </cols>

</xml_diff>

<commit_message>
In the “FVS_PlotInit” tab in the databaseDescription.xlsx file, the “DataType” field for StandPlot_ID was blank, yielding NA values and causing upload crashed. It has been re-specified to "Text".
git-svn-id: svn+ssh://svn.code.sf.net/p/open-fvs/code/rFVS@3212 90b89b48-9230-0de4-5065-812dd12741b8
</commit_message>
<xml_diff>
--- a/shinyFVSOnlineDev/databaseDescription.xlsx
+++ b/shinyFVSOnlineDev/databaseDescription.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FVS\Project_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Open-FVS\rFVS\shinyFVSOnlineDev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB187F7-4374-427C-9EE8-DAF1B571DA06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB14DBD-B35F-41D6-8A99-955FE94C813D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="47" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTableDescriptions" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4852" uniqueCount="1918">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4853" uniqueCount="1918">
   <si>
     <t>Table</t>
   </si>
@@ -10136,7 +10136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E862E947-F1E6-43BF-9C6E-9E8C99A65D26}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -22307,7 +22307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:AMK70"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -23310,8 +23310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:AMK71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23400,7 +23400,9 @@
       <c r="B6" s="7" t="s">
         <v>1695</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>103</v>
+      </c>
       <c r="D6" s="7" t="s">
         <v>1696</v>
       </c>
@@ -24772,7 +24774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:AMK30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -25215,7 +25217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrected the volume definitions in the CmpStdStk_East table
git-svn-id: svn+ssh://svn.code.sf.net/p/open-fvs/code/rFVS@3230 90b89b48-9230-0de4-5065-812dd12741b8
</commit_message>
<xml_diff>
--- a/shinyFVSOnlineDev/databaseDescription.xlsx
+++ b/shinyFVSOnlineDev/databaseDescription.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\FVS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Open-FVS\rFVS\shinyFVSOnlineDev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C1C81D-DD8C-4F79-8349-6388CB3E6DE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF3BA8E-337B-4DF8-8266-8152515D42D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="48" activeTab="51" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTableDescriptions" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4791" uniqueCount="1903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4791" uniqueCount="1915">
   <si>
     <t>Table</t>
   </si>
@@ -5875,6 +5875,42 @@
   </si>
   <si>
     <t>View_DWN</t>
+  </si>
+  <si>
+    <t>Weighted average of the sawlog cubic foot volume (cuft) of live trees in the diameter class at the beginning of the cycle</t>
+  </si>
+  <si>
+    <t>Weighted average of the sawlog  cubic foot volume (cuft) of live trees in the diameter class that died during that FVS cycle</t>
+  </si>
+  <si>
+    <t>Weighted average of the sawlog  cubic foot volume (cuft) of harvested live trees in the diameter class</t>
+  </si>
+  <si>
+    <t>Weighted average of the sawlog  cubic foot volume (cuft)  of live trees in the diameter class at the end of the cycle, following all harvests</t>
+  </si>
+  <si>
+    <t>Weighted average of the merchantable (sawlog and pulpwood) cubic foot volume (cuft) of live trees in the diameter class at the beginning of the cycle</t>
+  </si>
+  <si>
+    <t>Weighted average of the merchantible (sawlog and pulpwood) cubic foot volume (cuft) of live trees in the diameter class that died during that FVS cycle</t>
+  </si>
+  <si>
+    <t>Weighted average of the merchantable (sawlog and pulpwood) cubic foot volume (cuft)  of harvested live trees in the diameter class</t>
+  </si>
+  <si>
+    <t>Weighted average of the merchantable (sawlog and pulpwood) cubic foot volume (cuft)  of live trees in the diameter class at the end of the cycle, following all harvests</t>
+  </si>
+  <si>
+    <t>Weighted average of the boardfoot sawlog volume (bdft) of live trees in the diameter class at the beginning of the cycle</t>
+  </si>
+  <si>
+    <t>Weighted average of the boardfoot sawlog volume (bdft) of live trees in the diameter class that died during that FVS cycle</t>
+  </si>
+  <si>
+    <t>Weighted average of the boardfoot sawlog volume (bdft) of harvested live trees in the diameter class</t>
+  </si>
+  <si>
+    <t>Weighted average of the boardfoot sawlog volume (bdft) of live trees in the diameter class at the end of the cycle, following all harvests</t>
   </si>
 </sst>
 </file>
@@ -8973,8 +9009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AMK31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10067,7 +10103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B47B84-FCA3-4C5C-87A1-540887727794}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -21476,13 +21512,19 @@
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25291907-6267-4012-A960-BDDBFF4A876F}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="119.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
@@ -21681,172 +21723,244 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>466</v>
+      <c r="A15" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>496</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>1876</v>
+      <c r="D15" s="4" t="s">
+        <v>1903</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>469</v>
+      <c r="A16" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>499</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>1877</v>
+      <c r="D16" s="4" t="s">
+        <v>1904</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>472</v>
+      <c r="A17" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>502</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>1878</v>
+      <c r="D17" s="4" t="s">
+        <v>1905</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>475</v>
+      <c r="A18" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>505</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>1879</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="D18" s="4" t="s">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>1880</v>
+      <c r="B19" s="7" t="s">
+        <v>1853</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>1881</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="D19" s="4" t="s">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>1860</v>
+      <c r="B20" s="7" t="s">
+        <v>1855</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>1882</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="D20" s="4" t="s">
+        <v>1908</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>1862</v>
+      <c r="B21" s="7" t="s">
+        <v>1856</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>1883</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="D21" s="4" t="s">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>1864</v>
+      <c r="B22" s="7" t="s">
+        <v>1858</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>1884</v>
+      <c r="D22" s="7" t="s">
+        <v>1910</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>484</v>
+      <c r="A23" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>509</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>1885</v>
+      <c r="D23" s="4" t="s">
+        <v>1911</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>487</v>
+      <c r="A24" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>512</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>1886</v>
+      <c r="D24" s="4" t="s">
+        <v>1912</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>490</v>
+      <c r="A25" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>515</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>1887</v>
+      <c r="D25" s="4" t="s">
+        <v>1913</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>493</v>
+      <c r="A26" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>518</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>1888</v>
-      </c>
+      <c r="D26" s="4" t="s">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FVS_Treelist_East was missing from the databaseDescription.xlsx file. It was added and the volume definition differentiated between that and the regular FVS_Treelist table.
git-svn-id: svn+ssh://svn.code.sf.net/p/open-fvs/code/rFVS@3266 90b89b48-9230-0de4-5065-812dd12741b8
</commit_message>
<xml_diff>
--- a/shinyFVSOnlineDev/databaseDescription.xlsx
+++ b/shinyFVSOnlineDev/databaseDescription.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Open-FVS\rFVS\shinyFVSOnlineDev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\FVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE377869-CE60-49E5-A29F-FE70FED499AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44019E94-EAAE-4822-84AC-9F193B73E703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTableDescriptions" sheetId="1" r:id="rId1"/>
@@ -25,55 +25,56 @@
     <sheet name="FVS_DM_Spp_Sum" sheetId="9" r:id="rId10"/>
     <sheet name="FVS_DM_Sz_Sum" sheetId="10" r:id="rId11"/>
     <sheet name="FVS_Treelist" sheetId="11" r:id="rId12"/>
-    <sheet name="FVS_Cutlist" sheetId="12" r:id="rId13"/>
-    <sheet name="FVS_ATRTList" sheetId="13" r:id="rId14"/>
-    <sheet name="StdStk" sheetId="14" r:id="rId15"/>
-    <sheet name="StdStk_East" sheetId="15" r:id="rId16"/>
-    <sheet name="FVS_Carbon" sheetId="16" r:id="rId17"/>
-    <sheet name="FVS_Consumption" sheetId="17" r:id="rId18"/>
-    <sheet name="FVS_Hrv_Carbon" sheetId="18" r:id="rId19"/>
-    <sheet name="FVS_Fuels" sheetId="19" r:id="rId20"/>
-    <sheet name="FVS_Potfire" sheetId="20" r:id="rId21"/>
-    <sheet name="FVS_Potfire_East" sheetId="21" r:id="rId22"/>
-    <sheet name="FVS_BurnReport" sheetId="22" r:id="rId23"/>
-    <sheet name="FVS_Mortality" sheetId="23" r:id="rId24"/>
-    <sheet name="FVS_Down_Wood_Cov" sheetId="24" r:id="rId25"/>
-    <sheet name="FVS_Down_Wood_Vol" sheetId="25" r:id="rId26"/>
-    <sheet name="FVS_CanProfile" sheetId="26" r:id="rId27"/>
-    <sheet name="FVS_SnagSum" sheetId="27" r:id="rId28"/>
-    <sheet name="FVS_SnagDet" sheetId="28" r:id="rId29"/>
-    <sheet name="FVS_StrClass" sheetId="29" r:id="rId30"/>
-    <sheet name="FVS_CalibStats" sheetId="30" r:id="rId31"/>
-    <sheet name="FVS_Climate" sheetId="31" r:id="rId32"/>
-    <sheet name="FVS_EconSummary" sheetId="32" r:id="rId33"/>
-    <sheet name="FVS_EconHarvestValue" sheetId="33" r:id="rId34"/>
-    <sheet name="FVS_RD_Sum" sheetId="34" r:id="rId35"/>
-    <sheet name="FVS_RD_Det" sheetId="35" r:id="rId36"/>
-    <sheet name="FVS_RD_Beetle" sheetId="36" r:id="rId37"/>
-    <sheet name="FVS_Stats_Species" sheetId="37" r:id="rId38"/>
-    <sheet name="FVS_Stats_Stand" sheetId="38" r:id="rId39"/>
-    <sheet name="FVS_Regen_Sprouts" sheetId="39" r:id="rId40"/>
-    <sheet name="FVS_Regen_SitePrep" sheetId="40" r:id="rId41"/>
-    <sheet name="FVS_Regen_HabType" sheetId="41" r:id="rId42"/>
-    <sheet name="FVS_Regen_Tally" sheetId="42" r:id="rId43"/>
-    <sheet name="FVS_Regen_Ingrowth" sheetId="43" r:id="rId44"/>
-    <sheet name="InputTableDescriptions" sheetId="44" r:id="rId45"/>
-    <sheet name="FVS_GroupAddFilesAndKeywords" sheetId="45" r:id="rId46"/>
-    <sheet name="FVS_StandInit" sheetId="46" r:id="rId47"/>
-    <sheet name="FVS_PlotInit" sheetId="47" r:id="rId48"/>
-    <sheet name="FVS_TreeInit" sheetId="48" r:id="rId49"/>
-    <sheet name="CmpMetaData" sheetId="49" r:id="rId50"/>
-    <sheet name="CmpStdStk" sheetId="54" r:id="rId51"/>
-    <sheet name="CmpStdStk_East" sheetId="55" r:id="rId52"/>
-    <sheet name="CmpSummary" sheetId="50" r:id="rId53"/>
-    <sheet name="CmpSummary_East" sheetId="51" r:id="rId54"/>
-    <sheet name="CmpSummary2" sheetId="52" r:id="rId55"/>
-    <sheet name="CmpSummary2_East" sheetId="53" r:id="rId56"/>
+    <sheet name="FVS_Treelist_East" sheetId="57" r:id="rId13"/>
+    <sheet name="FVS_Cutlist" sheetId="12" r:id="rId14"/>
+    <sheet name="FVS_ATRTList" sheetId="13" r:id="rId15"/>
+    <sheet name="StdStk" sheetId="14" r:id="rId16"/>
+    <sheet name="StdStk_East" sheetId="15" r:id="rId17"/>
+    <sheet name="FVS_Carbon" sheetId="16" r:id="rId18"/>
+    <sheet name="FVS_Consumption" sheetId="17" r:id="rId19"/>
+    <sheet name="FVS_Hrv_Carbon" sheetId="18" r:id="rId20"/>
+    <sheet name="FVS_Fuels" sheetId="19" r:id="rId21"/>
+    <sheet name="FVS_Potfire" sheetId="20" r:id="rId22"/>
+    <sheet name="FVS_Potfire_East" sheetId="21" r:id="rId23"/>
+    <sheet name="FVS_BurnReport" sheetId="22" r:id="rId24"/>
+    <sheet name="FVS_Mortality" sheetId="23" r:id="rId25"/>
+    <sheet name="FVS_Down_Wood_Cov" sheetId="24" r:id="rId26"/>
+    <sheet name="FVS_Down_Wood_Vol" sheetId="25" r:id="rId27"/>
+    <sheet name="FVS_CanProfile" sheetId="26" r:id="rId28"/>
+    <sheet name="FVS_SnagSum" sheetId="27" r:id="rId29"/>
+    <sheet name="FVS_SnagDet" sheetId="28" r:id="rId30"/>
+    <sheet name="FVS_StrClass" sheetId="29" r:id="rId31"/>
+    <sheet name="FVS_CalibStats" sheetId="30" r:id="rId32"/>
+    <sheet name="FVS_Climate" sheetId="31" r:id="rId33"/>
+    <sheet name="FVS_EconSummary" sheetId="32" r:id="rId34"/>
+    <sheet name="FVS_EconHarvestValue" sheetId="33" r:id="rId35"/>
+    <sheet name="FVS_RD_Sum" sheetId="34" r:id="rId36"/>
+    <sheet name="FVS_RD_Det" sheetId="35" r:id="rId37"/>
+    <sheet name="FVS_RD_Beetle" sheetId="36" r:id="rId38"/>
+    <sheet name="FVS_Stats_Species" sheetId="37" r:id="rId39"/>
+    <sheet name="FVS_Stats_Stand" sheetId="38" r:id="rId40"/>
+    <sheet name="FVS_Regen_Sprouts" sheetId="39" r:id="rId41"/>
+    <sheet name="FVS_Regen_SitePrep" sheetId="40" r:id="rId42"/>
+    <sheet name="FVS_Regen_HabType" sheetId="41" r:id="rId43"/>
+    <sheet name="FVS_Regen_Tally" sheetId="42" r:id="rId44"/>
+    <sheet name="FVS_Regen_Ingrowth" sheetId="43" r:id="rId45"/>
+    <sheet name="InputTableDescriptions" sheetId="44" r:id="rId46"/>
+    <sheet name="FVS_GroupAddFilesAndKeywords" sheetId="45" r:id="rId47"/>
+    <sheet name="FVS_StandInit" sheetId="46" r:id="rId48"/>
+    <sheet name="FVS_PlotInit" sheetId="47" r:id="rId49"/>
+    <sheet name="FVS_TreeInit" sheetId="48" r:id="rId50"/>
+    <sheet name="CmpMetaData" sheetId="49" r:id="rId51"/>
+    <sheet name="CmpStdStk" sheetId="54" r:id="rId52"/>
+    <sheet name="CmpStdStk_East" sheetId="55" r:id="rId53"/>
+    <sheet name="CmpSummary" sheetId="50" r:id="rId54"/>
+    <sheet name="CmpSummary_East" sheetId="51" r:id="rId55"/>
+    <sheet name="CmpSummary2" sheetId="52" r:id="rId56"/>
+    <sheet name="CmpSummary2_East" sheetId="53" r:id="rId57"/>
   </sheets>
   <definedNames>
-    <definedName name="OLE_LINK3" localSheetId="16">FVS_Carbon!$D$5</definedName>
-    <definedName name="OLE_LINK3" localSheetId="14">StdStk!$D$5</definedName>
-    <definedName name="OLE_LINK3" localSheetId="15">StdStk_East!$D$5</definedName>
+    <definedName name="OLE_LINK3" localSheetId="17">FVS_Carbon!$D$5</definedName>
+    <definedName name="OLE_LINK3" localSheetId="15">StdStk!$D$5</definedName>
+    <definedName name="OLE_LINK3" localSheetId="16">StdStk_East!$D$5</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -85,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4791" uniqueCount="1927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4923" uniqueCount="1936">
   <si>
     <t>Table</t>
   </si>
@@ -5947,6 +5948,33 @@
   </si>
   <si>
     <t>Total Production Trees Per Acre</t>
+  </si>
+  <si>
+    <t>ScuFt</t>
+  </si>
+  <si>
+    <t>Sawlog Cubic Feet (cuft)</t>
+  </si>
+  <si>
+    <t>Total cubic foot volume per tree represented by the record. Since this is a per tree value it must be multiplied by the trees-per-acre value for the record in order to get the total cubic foot volume for the entire record.</t>
+  </si>
+  <si>
+    <t>Merchantable cubic foot volume (sawlog and pulpwood) per tree represented by the record. This is a net volume that has been reduced for defect. The defect percent applied is shown in Mdefect (see below). Since this is a per tree value it must be multiplied by the trees-per-acre value for the record in order to get the merchantable cubic foot volume for the entire record.</t>
+  </si>
+  <si>
+    <t>Board foot volume per tree represented by the record. This is a net volume that has been reduced for defect. The defect percent applied is shown in Bdefect (see below). Since this is a per tree value it must be multiplied by the trees-per-acre value for the record in order to get the board foot volume for the entire record.</t>
+  </si>
+  <si>
+    <t>Sawlog cubic foot volume per tree represented by the record. Since this is a per tree value it must be multiplied by the trees-per-acre value for the record in order to get the sawlog cubic foot volume for the entire record.</t>
+  </si>
+  <si>
+    <t>Merchantable cubic foot volume per tree represented by the record. This is a net volume that has been reduced for defect. The defect percent applied is shown in Mdefect (see below). Since this is a per tree value it must be multiplied by the trees-per-acre value for the record in order to get the merchatable cubic foot volume for the entire record.</t>
+  </si>
+  <si>
+    <t>Merchantable Cubic Feet (sawlog and pulpwood) (cuft)</t>
+  </si>
+  <si>
+    <t>FVS_Treelist_East</t>
   </si>
 </sst>
 </file>
@@ -6027,7 +6055,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6079,6 +6107,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6396,10 +6428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK49"/>
+  <dimension ref="A1:AMK50"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6499,308 +6531,316 @@
     </row>
     <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -7242,8 +7282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMK32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7563,7 +7603,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>160</v>
       </c>
@@ -7574,7 +7614,7 @@
         <v>123</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>409</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -7588,10 +7628,10 @@
         <v>123</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>1933</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>166</v>
       </c>
@@ -7602,7 +7642,7 @@
         <v>123</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>413</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -7710,6 +7750,476 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5317084B-D257-4148-A1E2-9AA631D18C6D}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>361</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>368</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>371</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>382</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>384</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>385</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>387</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>390</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>394</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
+        <v>396</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>397</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>399</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>1928</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>1932</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>1934</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>412</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>418</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="C28" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
+        <v>423</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>424</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="21" t="s">
+        <v>426</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>427</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
+        <v>432</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>433</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>434</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AMK32"/>
   <sheetViews>
@@ -8180,7 +8690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AMK32"/>
   <sheetViews>
@@ -8651,7 +9161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AMK31"/>
   <sheetViews>
@@ -9050,12 +9560,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AMK31"/>
   <sheetViews>
     <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9449,7 +9959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
@@ -9679,7 +10189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AMK20"/>
   <sheetViews>
@@ -9980,7 +10490,495 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B47B84-FCA3-4C5C-87A1-540887727794}">
+  <dimension ref="A1:B52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>1935</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>1894</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{7AB3B3FA-DB21-4485-8FF0-94D82696A62C}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{FD67315F-710E-429D-AC3A-EFB0DA00A9CA}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{0F3E2B57-13BB-4C0B-AB0A-F7381F24A750}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{6383CC25-65E8-4D42-AC60-B155A27F7B8A}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{EC1C21FE-116A-4076-851E-41352AF9B3DC}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{CD80295B-3795-4B63-943D-840133CA0420}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{9E4D5A88-AB08-4735-9E18-A880F8A8708D}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{DF3EDD72-0003-4ABA-8C56-FBC37753692A}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{27E9670D-9882-44DD-ABC9-A63360AC5CFA}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{B9510326-9C39-4D06-9A0C-48F77C49A871}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{1710F703-FCF8-472C-8FA7-A9AD17F07727}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{5EC4CA8F-D97F-45C7-8BE0-BD278A494CDB}"/>
+    <hyperlink ref="B18" r:id="rId13" xr:uid="{4B2B86F5-EA91-4974-B56A-A7AE4CA49F90}"/>
+    <hyperlink ref="B19" r:id="rId14" xr:uid="{AFAB471B-7A69-4DAF-8949-6A91B6FFFC07}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{EC5F9BC2-DE24-49D4-99A1-66790FF8F46E}"/>
+    <hyperlink ref="B20" r:id="rId16" xr:uid="{966CBB8C-2DCA-4E88-8C08-FD91CFA4CF5A}"/>
+    <hyperlink ref="B21" r:id="rId17" xr:uid="{FE12AEA1-A63F-48E8-961C-0C0D3A7680B8}"/>
+    <hyperlink ref="B22" r:id="rId18" xr:uid="{241045C4-0738-4B09-9B7B-0AD3DC3D3AEA}"/>
+    <hyperlink ref="B23" r:id="rId19" xr:uid="{9AD1ECAE-5875-48F8-9801-C085F1AEFAF6}"/>
+    <hyperlink ref="B24" r:id="rId20" xr:uid="{362AFE7D-79AA-40DC-A686-48016BC45904}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{C19A4BE5-3F02-4770-ADAF-84DD7020B8E4}"/>
+    <hyperlink ref="B26" r:id="rId22" xr:uid="{D37E3734-4FFB-419A-AF79-BC8B51342916}"/>
+    <hyperlink ref="B27" r:id="rId23" xr:uid="{0AED6549-C701-4467-B2CF-D0F12936BCFA}"/>
+    <hyperlink ref="B28" r:id="rId24" xr:uid="{CBD7478E-FA69-48CC-BAB6-4DD1762834BB}"/>
+    <hyperlink ref="B29" r:id="rId25" xr:uid="{38A818A1-6A24-422D-9BA5-FD5006E36165}"/>
+    <hyperlink ref="B31" r:id="rId26" xr:uid="{E1108ECA-32E2-4C4D-8D77-D7C6F6F8B2CC}"/>
+    <hyperlink ref="B32" r:id="rId27" xr:uid="{751C0E1B-99E4-473F-8A79-2BDF7BE4D92E}"/>
+    <hyperlink ref="B33" r:id="rId28" xr:uid="{90EE99D2-FD00-4A8D-95C4-C88D5374FADB}"/>
+    <hyperlink ref="B34" r:id="rId29" xr:uid="{461D5C4F-BE00-48A0-B09F-50D971584017}"/>
+    <hyperlink ref="B35" r:id="rId30" xr:uid="{85E179D0-9627-4E94-BC24-AB71A69C4BD2}"/>
+    <hyperlink ref="B36" r:id="rId31" xr:uid="{5FEA2701-7CC0-477A-A972-7390B3A39071}"/>
+    <hyperlink ref="B37" r:id="rId32" xr:uid="{1D8A030A-02A2-4883-8176-4714B2BC9DEB}"/>
+    <hyperlink ref="B38" r:id="rId33" xr:uid="{0C79D643-E011-4053-8C54-7D6E60A04471}"/>
+    <hyperlink ref="B39" r:id="rId34" xr:uid="{38FDC458-9EC3-492C-BBBA-8F4DAEC13C85}"/>
+    <hyperlink ref="B40" r:id="rId35" xr:uid="{7AC6C4FD-5AE1-4C9D-9E8F-7D69628B469D}"/>
+    <hyperlink ref="B41" r:id="rId36" xr:uid="{9D356455-1C91-485E-9CC7-3D8E5D7554A5}"/>
+    <hyperlink ref="B42" r:id="rId37" xr:uid="{189B0F9F-2F20-44F9-A7F7-81494AB2D9E4}"/>
+    <hyperlink ref="B43" r:id="rId38" xr:uid="{6BBB86E0-F72B-4740-BE1D-D1B5F4E16E45}"/>
+    <hyperlink ref="B30" r:id="rId39" xr:uid="{46745855-CDC8-40D6-9BCB-5F89CA72C370}"/>
+    <hyperlink ref="B14" r:id="rId40" xr:uid="{A98E5611-4E92-4F20-9FB2-76FD64B947F4}"/>
+    <hyperlink ref="B15" r:id="rId41" xr:uid="{1A2CF046-74D2-4C9C-A284-8595C354829E}"/>
+    <hyperlink ref="B44" r:id="rId42" xr:uid="{8993B95C-A6A7-4D84-A33B-CBDA33E96DC8}"/>
+    <hyperlink ref="B45" r:id="rId43" xr:uid="{8033814E-8AE1-4DB9-AD90-41BDFD44F710}"/>
+    <hyperlink ref="B46" r:id="rId44" xr:uid="{1EECDFFA-6163-462D-B730-9709DA44E032}"/>
+    <hyperlink ref="B47" r:id="rId45" xr:uid="{B9709C33-4C81-49DC-8010-29CF038C2BDB}"/>
+    <hyperlink ref="B48" r:id="rId46" xr:uid="{B3F46F6A-FAE0-4518-9EBD-610F8846F0FA}"/>
+    <hyperlink ref="B49" r:id="rId47" xr:uid="{A8BDFBF6-7676-4861-BB8D-9F54AFBEFC2E}"/>
+    <hyperlink ref="B50" r:id="rId48" xr:uid="{AA8B3B75-E22E-4541-B8D6-882ACD066A6B}"/>
+    <hyperlink ref="B51" r:id="rId49" xr:uid="{209D07D0-08A9-435E-9A9A-906197318F8E}"/>
+    <hyperlink ref="B52" r:id="rId50" xr:uid="{3AC97172-A4DB-408E-BCAE-9DE94D5E632B}"/>
+    <hyperlink ref="B12" r:id="rId51" xr:uid="{E47B01FB-34E0-4BD6-AF62-E1A432DF30C6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
@@ -10144,486 +11142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B47B84-FCA3-4C5C-87A1-540887727794}">
-  <dimension ref="A1:B51"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="96.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>1887</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>1889</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>1889</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>1891</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>1891</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>1891</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>1889</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>1889</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>1892</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>1892</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>1889</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>1894</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>1895</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>1896</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>1896</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>1897</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>1897</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>1897</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>1889</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>1889</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>1898</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>1898</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>1898</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>1898</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>1898</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B49" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>1899</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>1900</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{7AB3B3FA-DB21-4485-8FF0-94D82696A62C}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{FD67315F-710E-429D-AC3A-EFB0DA00A9CA}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{0F3E2B57-13BB-4C0B-AB0A-F7381F24A750}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{6383CC25-65E8-4D42-AC60-B155A27F7B8A}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{EC1C21FE-116A-4076-851E-41352AF9B3DC}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{CD80295B-3795-4B63-943D-840133CA0420}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{9E4D5A88-AB08-4735-9E18-A880F8A8708D}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{DF3EDD72-0003-4ABA-8C56-FBC37753692A}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{27E9670D-9882-44DD-ABC9-A63360AC5CFA}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{B9510326-9C39-4D06-9A0C-48F77C49A871}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{1710F703-FCF8-472C-8FA7-A9AD17F07727}"/>
-    <hyperlink ref="B15" r:id="rId12" xr:uid="{5EC4CA8F-D97F-45C7-8BE0-BD278A494CDB}"/>
-    <hyperlink ref="B17" r:id="rId13" xr:uid="{4B2B86F5-EA91-4974-B56A-A7AE4CA49F90}"/>
-    <hyperlink ref="B18" r:id="rId14" xr:uid="{AFAB471B-7A69-4DAF-8949-6A91B6FFFC07}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{EC5F9BC2-DE24-49D4-99A1-66790FF8F46E}"/>
-    <hyperlink ref="B19" r:id="rId16" xr:uid="{966CBB8C-2DCA-4E88-8C08-FD91CFA4CF5A}"/>
-    <hyperlink ref="B20" r:id="rId17" xr:uid="{FE12AEA1-A63F-48E8-961C-0C0D3A7680B8}"/>
-    <hyperlink ref="B21" r:id="rId18" xr:uid="{241045C4-0738-4B09-9B7B-0AD3DC3D3AEA}"/>
-    <hyperlink ref="B22" r:id="rId19" xr:uid="{9AD1ECAE-5875-48F8-9801-C085F1AEFAF6}"/>
-    <hyperlink ref="B23" r:id="rId20" xr:uid="{362AFE7D-79AA-40DC-A686-48016BC45904}"/>
-    <hyperlink ref="B24" r:id="rId21" xr:uid="{C19A4BE5-3F02-4770-ADAF-84DD7020B8E4}"/>
-    <hyperlink ref="B25" r:id="rId22" xr:uid="{D37E3734-4FFB-419A-AF79-BC8B51342916}"/>
-    <hyperlink ref="B26" r:id="rId23" xr:uid="{0AED6549-C701-4467-B2CF-D0F12936BCFA}"/>
-    <hyperlink ref="B27" r:id="rId24" xr:uid="{CBD7478E-FA69-48CC-BAB6-4DD1762834BB}"/>
-    <hyperlink ref="B28" r:id="rId25" xr:uid="{38A818A1-6A24-422D-9BA5-FD5006E36165}"/>
-    <hyperlink ref="B30" r:id="rId26" xr:uid="{E1108ECA-32E2-4C4D-8D77-D7C6F6F8B2CC}"/>
-    <hyperlink ref="B31" r:id="rId27" xr:uid="{751C0E1B-99E4-473F-8A79-2BDF7BE4D92E}"/>
-    <hyperlink ref="B32" r:id="rId28" xr:uid="{90EE99D2-FD00-4A8D-95C4-C88D5374FADB}"/>
-    <hyperlink ref="B33" r:id="rId29" xr:uid="{461D5C4F-BE00-48A0-B09F-50D971584017}"/>
-    <hyperlink ref="B34" r:id="rId30" xr:uid="{85E179D0-9627-4E94-BC24-AB71A69C4BD2}"/>
-    <hyperlink ref="B35" r:id="rId31" xr:uid="{5FEA2701-7CC0-477A-A972-7390B3A39071}"/>
-    <hyperlink ref="B36" r:id="rId32" xr:uid="{1D8A030A-02A2-4883-8176-4714B2BC9DEB}"/>
-    <hyperlink ref="B37" r:id="rId33" xr:uid="{0C79D643-E011-4053-8C54-7D6E60A04471}"/>
-    <hyperlink ref="B38" r:id="rId34" xr:uid="{38FDC458-9EC3-492C-BBBA-8F4DAEC13C85}"/>
-    <hyperlink ref="B39" r:id="rId35" xr:uid="{7AC6C4FD-5AE1-4C9D-9E8F-7D69628B469D}"/>
-    <hyperlink ref="B40" r:id="rId36" xr:uid="{9D356455-1C91-485E-9CC7-3D8E5D7554A5}"/>
-    <hyperlink ref="B41" r:id="rId37" xr:uid="{189B0F9F-2F20-44F9-A7F7-81494AB2D9E4}"/>
-    <hyperlink ref="B42" r:id="rId38" xr:uid="{6BBB86E0-F72B-4740-BE1D-D1B5F4E16E45}"/>
-    <hyperlink ref="B29" r:id="rId39" xr:uid="{46745855-CDC8-40D6-9BCB-5F89CA72C370}"/>
-    <hyperlink ref="B13" r:id="rId40" xr:uid="{A98E5611-4E92-4F20-9FB2-76FD64B947F4}"/>
-    <hyperlink ref="B14" r:id="rId41" xr:uid="{1A2CF046-74D2-4C9C-A284-8595C354829E}"/>
-    <hyperlink ref="B43" r:id="rId42" xr:uid="{8993B95C-A6A7-4D84-A33B-CBDA33E96DC8}"/>
-    <hyperlink ref="B44" r:id="rId43" xr:uid="{8033814E-8AE1-4DB9-AD90-41BDFD44F710}"/>
-    <hyperlink ref="B45" r:id="rId44" xr:uid="{1EECDFFA-6163-462D-B730-9709DA44E032}"/>
-    <hyperlink ref="B46" r:id="rId45" xr:uid="{B9709C33-4C81-49DC-8010-29CF038C2BDB}"/>
-    <hyperlink ref="B47" r:id="rId46" xr:uid="{B3F46F6A-FAE0-4518-9EBD-610F8846F0FA}"/>
-    <hyperlink ref="B48" r:id="rId47" xr:uid="{A8BDFBF6-7676-4861-BB8D-9F54AFBEFC2E}"/>
-    <hyperlink ref="B49" r:id="rId48" xr:uid="{AA8B3B75-E22E-4541-B8D6-882ACD066A6B}"/>
-    <hyperlink ref="B50" r:id="rId49" xr:uid="{209D07D0-08A9-435E-9A9A-906197318F8E}"/>
-    <hyperlink ref="B51" r:id="rId50" xr:uid="{3AC97172-A4DB-408E-BCAE-9DE94D5E632B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AMK23"/>
   <sheetViews>
@@ -10968,7 +11487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AMK30"/>
   <sheetViews>
@@ -11411,7 +11930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:AMK22"/>
   <sheetViews>
@@ -11742,7 +12261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:AMK24"/>
   <sheetViews>
@@ -12101,7 +12620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:AMK21"/>
   <sheetViews>
@@ -12418,7 +12937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
@@ -12693,7 +13212,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:AMK20"/>
   <sheetViews>
@@ -12995,7 +13514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:AMK8"/>
   <sheetViews>
@@ -13130,7 +13649,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:AMK19"/>
   <sheetViews>
@@ -13411,253 +13930,6 @@
       </c>
       <c r="D19" s="7" t="s">
         <v>956</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <dimension ref="A1:AMK16"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.88671875" style="7"/>
-    <col min="2" max="2" width="19" style="7" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="7"/>
-    <col min="4" max="4" width="49.6640625" style="7" customWidth="1"/>
-    <col min="5" max="1025" width="10.88671875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>958</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>959</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>961</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>962</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>964</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>965</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>967</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>968</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>970</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>971</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>973</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>974</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>975</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>976</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>977</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>978</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>980</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>981</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>983</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>984</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>986</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>987</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>988</v>
       </c>
     </row>
   </sheetData>
@@ -13872,6 +14144,253 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <dimension ref="A1:AMK16"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.88671875" style="7"/>
+    <col min="2" max="2" width="19" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" style="7"/>
+    <col min="4" max="4" width="49.6640625" style="7" customWidth="1"/>
+    <col min="5" max="1025" width="10.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>958</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>959</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>961</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>962</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>964</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>965</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>967</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>968</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>970</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>971</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>973</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>975</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>976</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>977</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>978</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>980</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>981</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>986</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>987</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>988</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:AMK35"/>
   <sheetViews>
@@ -14384,7 +14903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
@@ -14547,7 +15066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:AMK14"/>
   <sheetViews>
@@ -14765,7 +15284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:AMK20"/>
   <sheetViews>
@@ -15068,7 +15587,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:AMK16"/>
   <sheetViews>
@@ -15314,7 +15833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:AMK16"/>
   <sheetViews>
@@ -15561,7 +16080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:AMK23"/>
   <sheetViews>
@@ -15906,7 +16425,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:AMK33"/>
   <sheetViews>
@@ -16391,7 +16910,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -16530,223 +17049,6 @@
       </c>
       <c r="D9" s="7" t="s">
         <v>1385</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
-  <dimension ref="A1:D14"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="2" width="42.109375" customWidth="1"/>
-    <col min="4" max="4" width="77.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>1386</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>1386</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>1388</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>1389</v>
-      </c>
-      <c r="C6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>1390</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>1391</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>1392</v>
-      </c>
-      <c r="C7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>1393</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>1394</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>1395</v>
-      </c>
-      <c r="C8" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>1396</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>1397</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>1398</v>
-      </c>
-      <c r="C9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>1399</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>1400</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>1401</v>
-      </c>
-      <c r="C10" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>1402</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>1403</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>1404</v>
-      </c>
-      <c r="C11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>1405</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>1406</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>1407</v>
-      </c>
-      <c r="C12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>1408</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>1409</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>1410</v>
-      </c>
-      <c r="C13" t="s">
-        <v>123</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>1412</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>1413</v>
-      </c>
-      <c r="C14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>1414</v>
       </c>
     </row>
   </sheetData>
@@ -17202,6 +17504,223 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" customWidth="1"/>
+    <col min="4" max="4" width="77.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1404</v>
+      </c>
+      <c r="C11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -17320,7 +17839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -17467,7 +17986,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -17586,7 +18105,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -17803,7 +18322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
@@ -17969,7 +18488,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:AMK5"/>
   <sheetViews>
@@ -18030,7 +18549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:AMK4"/>
   <sheetViews>
@@ -18108,7 +18627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:AMK70"/>
   <sheetViews>
@@ -19111,7 +19630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:AMK71"/>
   <sheetViews>
@@ -20120,449 +20639,6 @@
       </c>
       <c r="D71" s="15" t="s">
         <v>1690</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
-  <dimension ref="A1:AMK30"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="53.6640625" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.5546875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>1691</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
-        <v>1504</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>1691</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>1506</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>1692</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>1693</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>1697</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>1695</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>1699</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>1694</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>1698</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>1701</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>1703</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>1704</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>1705</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>1706</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>1707</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>1708</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>366</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>1709</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>381</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>1710</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>1711</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>384</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>385</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>1712</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>387</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>1715</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>391</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>1716</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>1718</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>1719</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>1720</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>1721</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>1722</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>1724</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>1725</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>1726</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>1727</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>1728</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>1729</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>1730</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>1731</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
-        <v>1732</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>1733</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>1734</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
-        <v>1735</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>1736</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>1731</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
-        <v>1737</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>1738</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>1734</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="16" t="s">
-        <v>368</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>1739</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>1740</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
-        <v>1741</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>1742</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>1743</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>1744</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>1745</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="16" t="s">
-        <v>751</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>1746</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>1747</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
-        <v>1549</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>1748</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>1749</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
-        <v>1541</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>1542</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
-        <v>1751</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>1752</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>1753</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>1755</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>1756</v>
       </c>
     </row>
   </sheetData>
@@ -21019,6 +21095,449 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
+  <dimension ref="A1:AMK30"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="53.6640625" style="2" customWidth="1"/>
+    <col min="5" max="1025" width="8.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1692</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>1697</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>1699</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>1701</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1704</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>1709</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1713</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>1721</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>1725</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>1733</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
+        <v>368</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="16" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
+        <v>751</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>1746</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>1753</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>1755</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -21170,7 +21689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25504409-66C9-4165-AAA9-4F3B04E11F18}">
   <dimension ref="A1:D26"/>
   <sheetViews>
@@ -21555,7 +22074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25291907-6267-4012-A960-BDDBFF4A876F}">
   <dimension ref="A1:D40"/>
   <sheetViews>
@@ -22012,7 +22531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
@@ -22360,7 +22879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:D1048576"/>
   <sheetViews>
@@ -22708,7 +23227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <dimension ref="A1:AMK23"/>
   <sheetViews>
@@ -23057,7 +23576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <dimension ref="A1:AMK23"/>
   <sheetViews>
@@ -23410,7 +23929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMK30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added in the View_DWN table for the Describe Tables dropdown list
git-svn-id: svn+ssh://svn.code.sf.net/p/open-fvs/code/rFVS@3521 90b89b48-9230-0de4-5065-812dd12741b8
</commit_message>
<xml_diff>
--- a/shinyFVSOnlineDev/databaseDescription.xlsx
+++ b/shinyFVSOnlineDev/databaseDescription.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Open-FVS\rFVS\shinyFVSOnlineDev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\FVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7645C0CF-4F5A-48DF-AD81-A276064CC212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68A79D3-BC7B-441E-AF3E-2D30CDC564D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="42" activeTab="45" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTableDescriptions" sheetId="1" r:id="rId1"/>
@@ -71,6 +71,7 @@
     <sheet name="CmpSummary_East" sheetId="51" r:id="rId56"/>
     <sheet name="CmpSummary2" sheetId="52" r:id="rId57"/>
     <sheet name="CmpSummary2_East" sheetId="53" r:id="rId58"/>
+    <sheet name="View_DWN" sheetId="61" r:id="rId59"/>
   </sheets>
   <definedNames>
     <definedName name="OLE_LINK3" localSheetId="17">FVS_Carbon!$D$5</definedName>
@@ -87,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4981" uniqueCount="1960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5024" uniqueCount="1968">
   <si>
     <t>Table</t>
   </si>
@@ -6048,6 +6049,30 @@
   </si>
   <si>
     <t>FVS_Regen_Ingrow</t>
+  </si>
+  <si>
+    <t>Case_ID</t>
+  </si>
+  <si>
+    <t>DWD_Total_Cover</t>
+  </si>
+  <si>
+    <t>DWD_Total_Volume</t>
+  </si>
+  <si>
+    <t>Total cover of hard and soft down wood (%)</t>
+  </si>
+  <si>
+    <t>Reported in percent cover (%). The total columns estimate the total down wood cover (3” and larger) for hard and soft wood.</t>
+  </si>
+  <si>
+    <t>Total volume of soft and hard down wood (cuft/acre)</t>
+  </si>
+  <si>
+    <t>Reported in cuft/acre. The total estimates the total down wood volume for soft and hard decay class.</t>
+  </si>
+  <si>
+    <t>is a view of the total percent cover and cubic feet per acre volume of both soft and hard downed wood, pulled from the FVS_Down_Wood_Cov and FVS_Down_Wood_Vol tables</t>
   </si>
 </sst>
 </file>
@@ -6135,7 +6160,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6193,6 +6218,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -6509,10 +6537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK51"/>
+  <dimension ref="A1:AMK52"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6931,6 +6959,14 @@
       </c>
       <c r="B51" s="1" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>1967</v>
       </c>
     </row>
   </sheetData>
@@ -10585,7 +10621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B47B84-FCA3-4C5C-87A1-540887727794}">
   <dimension ref="A1:XFD53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -29636,8 +29672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29912,7 +29948,7 @@
   <dimension ref="A1:AMK20"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B20" sqref="B20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35021,7 +35057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -35326,8 +35362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:AMK70"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39230,7 +39266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -40622,6 +40658,274 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10766AA6-72AD-494C-B412-4045B85131AB}">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>1960</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>798</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>815</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>816</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1963</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>833</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>851</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>852</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1965</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="7"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="7"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="7"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMK30"/>

</xml_diff>